<commit_message>
Add Student.recruitment_note and modify tests
</commit_message>
<xml_diff>
--- a/edziennik/tests/test_files/test.xlsx
+++ b/edziennik/tests/test_files/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">Imię klienta</t>
   </si>
@@ -34,10 +34,13 @@
     <t xml:space="preserve">Nazwisko ucznia</t>
   </si>
   <si>
+    <t xml:space="preserve">grupa</t>
+  </si>
+  <si>
     <t xml:space="preserve">nr tel</t>
   </si>
   <si>
-    <t xml:space="preserve">notatka</t>
+    <t xml:space="preserve">notatka rekrutacyjna</t>
   </si>
   <si>
     <t xml:space="preserve">Arek</t>
@@ -49,6 +52,9 @@
     <t xml:space="preserve">Adam</t>
   </si>
   <si>
+    <t xml:space="preserve">jun1</t>
+  </si>
+  <si>
     <t xml:space="preserve">coś o Arku</t>
   </si>
   <si>
@@ -62,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ważna grupa2 AĄŁ</t>
   </si>
   <si>
     <t xml:space="preserve">nota o Izie Ąś</t>
@@ -79,6 +88,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,15 +170,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -190,45 +200,54 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>690506333</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>77722233</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>14</v>
+      <c r="G3" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>